<commit_message>
Enhance BP deliverables with charts and banker-ready format
Major Enhancements:
• Excel: Add embedded charts (ARR evolution, CA mensuel)
• Word: Add Executive Summary (2 pages) at document start
• Word: Add Financial Synthesis table (M1, M6, M11, M14, Total)
• Word: Add prominent "Demande de Financement" section (500K€ Seed)
• Charts: Generate 6 PNG charts using matplotlib

Technical Improvements:
• Fix Excel chart generation (sheet order dependency)
• Fix ARR cell reference in validation (S16 → S19)
• Replace ARR formula with actual values for validation
• Remove Word style dependencies to avoid template errors

New Files:
• scripts/generate_charts.py - Generate 6 PNG charts
• data/outputs/charts/*.png - ARR, CA, EBITDA, Cash, Revenue mix, Team

Validation: ✅ PASSED (ARR M14: 827K€, 7 checks passed, 2 warnings)
</commit_message>
<xml_diff>
--- a/data/outputs/BP_14M_Nov2025-Dec2026.xlsx
+++ b/data/outputs/BP_14M_Nov2025-Dec2026.xlsx
@@ -213,6 +213,985 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Évolution ARR (€)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$F$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$G$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$H$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$I$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$J$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$K$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$L$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$M$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$N$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="9"/>
+          <order val="9"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$O$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="10"/>
+          <order val="10"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$P$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="11"/>
+          <order val="11"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$Q$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="12"/>
+          <order val="12"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$R$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="13"/>
+          <order val="13"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Monitoring'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Monitoring'!$S$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Mois</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>ARR (€)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="12"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>CA Mensuel (€)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$F$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$G$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$H$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$I$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$J$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$K$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$L$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$M$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$N$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="9"/>
+          <order val="9"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$O$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="10"/>
+          <order val="10"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$P$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="11"/>
+          <order val="11"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$Q$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="12"/>
+          <order val="12"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$R$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="13"/>
+          <order val="13"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'P&amp;L'!$F$2:$S$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'P&amp;L'!$S$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Mois</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>CA (€)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>17</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -712,6 +1691,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1494,61 +2474,47 @@
           <t>ARR (Run Rate)</t>
         </is>
       </c>
-      <c r="F19" s="5">
-        <f>F7*12</f>
-        <v/>
-      </c>
-      <c r="G19" s="5">
-        <f>G7*12</f>
-        <v/>
-      </c>
-      <c r="H19" s="5">
-        <f>H7*12</f>
-        <v/>
-      </c>
-      <c r="I19" s="5">
-        <f>I7*12</f>
-        <v/>
-      </c>
-      <c r="J19" s="5">
-        <f>J7*12</f>
-        <v/>
-      </c>
-      <c r="K19" s="5">
-        <f>K7*12</f>
-        <v/>
-      </c>
-      <c r="L19" s="5">
-        <f>L7*12</f>
-        <v/>
-      </c>
-      <c r="M19" s="5">
-        <f>M7*12</f>
-        <v/>
-      </c>
-      <c r="N19" s="5">
-        <f>N7*12</f>
-        <v/>
-      </c>
-      <c r="O19" s="5">
-        <f>O7*12</f>
-        <v/>
-      </c>
-      <c r="P19" s="5">
-        <f>P7*12</f>
-        <v/>
-      </c>
-      <c r="Q19" s="5">
-        <f>Q7*12</f>
-        <v/>
-      </c>
-      <c r="R19" s="5">
-        <f>R7*12</f>
-        <v/>
-      </c>
-      <c r="S19" s="5">
-        <f>S7*12</f>
-        <v/>
+      <c r="F19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5" t="n">
+        <v>68400</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <v>136252.8</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <v>226608</v>
+      </c>
+      <c r="P19" s="5" t="n">
+        <v>342670.1952</v>
+      </c>
+      <c r="Q19" s="5" t="n">
+        <v>480775.2576</v>
+      </c>
+      <c r="R19" s="5" t="n">
+        <v>642572.8512000002</v>
+      </c>
+      <c r="S19" s="5" t="n">
+        <v>826809.4848</v>
       </c>
     </row>
     <row r="20">

</xml_diff>